<commit_message>
Fix error in DNPPE components in component table
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_basic_component_matrix.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_basic_component_matrix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="0" windowWidth="26440" windowHeight="15700" tabRatio="500" activeTab="3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="97">
   <si>
     <t>DGCC</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>Renamed file</t>
+  </si>
+  <si>
+    <t>Fixed error in DNPPE components</t>
   </si>
 </sst>
 </file>
@@ -376,8 +379,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -452,7 +457,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -480,6 +485,7 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -507,6 +513,7 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -846,7 +853,7 @@
     <sheetView topLeftCell="A2" workbookViewId="0">
       <pane ySplit="560" activePane="bottomLeft"/>
       <selection activeCell="O2" sqref="O2"/>
-      <selection pane="bottomLeft" activeCell="Q17" sqref="Q17"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1177,13 +1184,13 @@
         <v>43</v>
       </c>
       <c r="C7">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <v>12</v>
@@ -1220,7 +1227,7 @@
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="0"/>
-        <v>874.54321115599998</v>
+        <v>857.51666203100001</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -3986,8 +3993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4250,13 +4257,13 @@
         <v>43</v>
       </c>
       <c r="C6">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>12</v>
@@ -6959,10 +6966,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7087,6 +7094,17 @@
         <v>50</v>
       </c>
     </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="7">
+        <v>42371</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Revised (correct) specifications for BLL and PDPT; still waiting to verify S_DGCC
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_basic_component_matrix.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_basic_component_matrix.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="168">
   <si>
     <t>DGCC</t>
   </si>
@@ -317,18 +317,9 @@
     <t>Added class IP_MAG and a LPC class to calculate lyso species</t>
   </si>
   <si>
-    <t>DB_gen_type</t>
-  </si>
-  <si>
-    <t>Unique_species</t>
-  </si>
-  <si>
     <t>Adduct_hierarchy_lookup_class</t>
   </si>
   <si>
-    <t>Acyl_iteration</t>
-  </si>
-  <si>
     <t>Scytonemin</t>
   </si>
   <si>
@@ -528,6 +519,21 @@
   </si>
   <si>
     <t>Modified "Adduct_hierarchy_lookup_class" to index directly on the field names in the adduct ion hierarchy matrix</t>
+  </si>
+  <si>
+    <t>Changed the name of "DB_gen_type" to "DB_gen_compound_type" and changed the values to entries that convey more meaning</t>
+  </si>
+  <si>
+    <t>DB_gen_compound_type</t>
+  </si>
+  <si>
+    <t>DB_acyl_iteration</t>
+  </si>
+  <si>
+    <t>DB_unique_species</t>
+  </si>
+  <si>
+    <t>Fixed composition definitions of BLL, PDPT (still verifying PDPT &amp; waiting on verification for S_DGCC)</t>
   </si>
 </sst>
 </file>
@@ -1066,9 +1072,9 @@
   <dimension ref="A1:T101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane ySplit="1080" topLeftCell="A2" activePane="bottomLeft"/>
+      <pane ySplit="1080" topLeftCell="A52" activePane="bottomLeft"/>
       <selection activeCell="R3" sqref="R3"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1171,13 +1177,13 @@
         <v>44</v>
       </c>
       <c r="P2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Q2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R2" t="s">
-        <v>95</v>
+        <v>164</v>
       </c>
       <c r="S2" t="s">
         <v>43</v>
@@ -1236,7 +1242,7 @@
         <v>53</v>
       </c>
       <c r="R3" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" ref="S3:S15" si="0">B3*$B$1+C3*$C$1+D3*$D$1+E3*$E$1+F3*$F$1+G3*$G$1+H3*$H$1+I3*$I$1+J3*$J$1+K3*$K$1+L3*$L$1+M3*$M$1+N3*$N$1+O3*$O$1</f>
@@ -1296,7 +1302,7 @@
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="0"/>
@@ -1356,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S5" s="4">
         <f t="shared" si="0"/>
@@ -1416,7 +1422,7 @@
         <v>2</v>
       </c>
       <c r="R6" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S6" s="4">
         <f t="shared" si="0"/>
@@ -1476,7 +1482,7 @@
         <v>3</v>
       </c>
       <c r="R7" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S7" s="4">
         <f t="shared" si="0"/>
@@ -1536,7 +1542,7 @@
         <v>4</v>
       </c>
       <c r="R8" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" si="0"/>
@@ -1596,7 +1602,7 @@
         <v>5</v>
       </c>
       <c r="R9" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S9" s="4">
         <f t="shared" si="0"/>
@@ -1656,7 +1662,7 @@
         <v>6</v>
       </c>
       <c r="R10" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S10" s="4">
         <f t="shared" si="0"/>
@@ -1716,7 +1722,7 @@
         <v>92</v>
       </c>
       <c r="R11" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S11" s="4">
         <f t="shared" si="0"/>
@@ -1776,7 +1782,7 @@
         <v>7</v>
       </c>
       <c r="R12" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S12" s="4">
         <f t="shared" si="0"/>
@@ -1836,7 +1842,7 @@
         <v>8</v>
       </c>
       <c r="R13" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S13" s="4">
         <f t="shared" si="0"/>
@@ -1896,7 +1902,7 @@
         <v>58</v>
       </c>
       <c r="R14" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S14" s="4">
         <f t="shared" si="0"/>
@@ -1956,7 +1962,7 @@
         <v>9</v>
       </c>
       <c r="R15" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S15" s="4">
         <f t="shared" si="0"/>
@@ -2010,7 +2016,10 @@
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>160</v>
+        <v>157</v>
+      </c>
+      <c r="R16" t="s">
+        <v>157</v>
       </c>
       <c r="S16" s="4">
         <f>B16*$B$1+C16*$C$1+D16*$D$1+E16*$E$1+F16*$F$1+G16*$G$1+H16*$H$1+I16*$I$1+J16*$J$1+K16*$K$1+L16*$L$1</f>
@@ -2064,7 +2073,10 @@
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>160</v>
+        <v>157</v>
+      </c>
+      <c r="R17" t="s">
+        <v>157</v>
       </c>
       <c r="S17" s="4">
         <f>B17*$B$1+C17*$C$1+D17*$D$1+E17*$E$1+F17*$F$1+G17*$G$1+H17*$H$1+I17*$I$1+J17*$J$1+K17*$K$1+L17*$L$1</f>
@@ -2118,7 +2130,10 @@
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R18" t="s">
+        <v>158</v>
       </c>
       <c r="S18" s="4">
         <f t="shared" ref="S18:S81" si="1">B18*$B$1+C18*$C$1+D18*$D$1+E18*$E$1+F18*$F$1+G18*$G$1+H18*$H$1+I18*$I$1+J18*$J$1+K18*$K$1+L18*$L$1+M18*$M$1+N18*$N$1+O18*$O$1</f>
@@ -2172,7 +2187,10 @@
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R19" t="s">
+        <v>158</v>
       </c>
       <c r="S19" s="4">
         <f t="shared" si="1"/>
@@ -2226,7 +2244,10 @@
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R20" t="s">
+        <v>158</v>
       </c>
       <c r="S20" s="4">
         <f t="shared" si="1"/>
@@ -2280,7 +2301,10 @@
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R21" t="s">
+        <v>158</v>
       </c>
       <c r="S21" s="4">
         <f t="shared" si="1"/>
@@ -2334,7 +2358,10 @@
         <v>0</v>
       </c>
       <c r="P22" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R22" t="s">
+        <v>158</v>
       </c>
       <c r="S22" s="4">
         <f t="shared" si="1"/>
@@ -2388,7 +2415,10 @@
         <v>0</v>
       </c>
       <c r="P23" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R23" t="s">
+        <v>158</v>
       </c>
       <c r="S23" s="4">
         <f t="shared" si="1"/>
@@ -2442,7 +2472,10 @@
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R24" t="s">
+        <v>158</v>
       </c>
       <c r="S24" s="4">
         <f t="shared" si="1"/>
@@ -2496,7 +2529,10 @@
         <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R25" t="s">
+        <v>158</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="1"/>
@@ -2550,7 +2586,10 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R26" t="s">
+        <v>158</v>
       </c>
       <c r="S26" s="4">
         <f t="shared" si="1"/>
@@ -2604,7 +2643,10 @@
         <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R27" t="s">
+        <v>158</v>
       </c>
       <c r="S27" s="4">
         <f t="shared" si="1"/>
@@ -2658,7 +2700,10 @@
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="R28" t="s">
+        <v>158</v>
       </c>
       <c r="S28" s="4">
         <f t="shared" si="1"/>
@@ -2712,7 +2757,10 @@
         <v>0</v>
       </c>
       <c r="P29" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R29" t="s">
+        <v>159</v>
       </c>
       <c r="S29" s="4">
         <f t="shared" si="1"/>
@@ -2766,7 +2814,10 @@
         <v>0</v>
       </c>
       <c r="P30" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R30" t="s">
+        <v>159</v>
       </c>
       <c r="S30" s="4">
         <f t="shared" si="1"/>
@@ -2820,7 +2871,10 @@
         <v>0</v>
       </c>
       <c r="P31" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R31" t="s">
+        <v>159</v>
       </c>
       <c r="S31" s="4">
         <f t="shared" si="1"/>
@@ -2874,7 +2928,10 @@
         <v>0</v>
       </c>
       <c r="P32" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R32" t="s">
+        <v>159</v>
       </c>
       <c r="S32" s="4">
         <f t="shared" si="1"/>
@@ -2928,7 +2985,10 @@
         <v>0</v>
       </c>
       <c r="P33" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R33" t="s">
+        <v>159</v>
       </c>
       <c r="S33" s="4">
         <f t="shared" si="1"/>
@@ -2982,7 +3042,10 @@
         <v>0</v>
       </c>
       <c r="P34" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R34" t="s">
+        <v>159</v>
       </c>
       <c r="S34" s="4">
         <f t="shared" si="1"/>
@@ -3036,7 +3099,10 @@
         <v>0</v>
       </c>
       <c r="P35" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R35" t="s">
+        <v>159</v>
       </c>
       <c r="S35" s="4">
         <f t="shared" si="1"/>
@@ -3090,7 +3156,10 @@
         <v>0</v>
       </c>
       <c r="P36" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R36" t="s">
+        <v>159</v>
       </c>
       <c r="S36" s="4">
         <f t="shared" si="1"/>
@@ -3144,7 +3213,10 @@
         <v>0</v>
       </c>
       <c r="P37" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R37" t="s">
+        <v>159</v>
       </c>
       <c r="S37" s="4">
         <f t="shared" si="1"/>
@@ -3204,7 +3276,7 @@
         <v>20</v>
       </c>
       <c r="R38" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S38" s="4">
         <f t="shared" si="1"/>
@@ -3264,7 +3336,7 @@
         <v>58</v>
       </c>
       <c r="R39" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S39" s="4">
         <f t="shared" si="1"/>
@@ -3324,7 +3396,7 @@
         <v>58</v>
       </c>
       <c r="R40" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S40" s="4">
         <f t="shared" si="1"/>
@@ -3384,7 +3456,7 @@
         <v>58</v>
       </c>
       <c r="R41" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S41" s="4">
         <f t="shared" si="1"/>
@@ -3444,7 +3516,7 @@
         <v>58</v>
       </c>
       <c r="R42" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S42" s="4">
         <f t="shared" si="1"/>
@@ -3504,7 +3576,7 @@
         <v>58</v>
       </c>
       <c r="R43" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S43" s="4">
         <f t="shared" si="1"/>
@@ -3564,7 +3636,7 @@
         <v>58</v>
       </c>
       <c r="R44" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S44" s="4">
         <f t="shared" si="1"/>
@@ -3624,7 +3696,7 @@
         <v>58</v>
       </c>
       <c r="R45" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S45" s="4">
         <f t="shared" si="1"/>
@@ -3684,7 +3756,7 @@
         <v>58</v>
       </c>
       <c r="R46" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S46" s="4">
         <f t="shared" si="1"/>
@@ -3744,7 +3816,7 @@
         <v>58</v>
       </c>
       <c r="R47" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S47" s="4">
         <f t="shared" si="1"/>
@@ -3804,7 +3876,7 @@
         <v>58</v>
       </c>
       <c r="R48" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S48" s="4">
         <f t="shared" si="1"/>
@@ -3864,7 +3936,7 @@
         <v>58</v>
       </c>
       <c r="R49" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S49" s="4">
         <f t="shared" si="1"/>
@@ -3924,7 +3996,7 @@
         <v>58</v>
       </c>
       <c r="R50" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S50" s="4">
         <f t="shared" si="1"/>
@@ -3984,7 +4056,7 @@
         <v>58</v>
       </c>
       <c r="R51" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S51" s="4">
         <f t="shared" si="1"/>
@@ -4044,7 +4116,7 @@
         <v>58</v>
       </c>
       <c r="R52" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S52" s="4">
         <f t="shared" si="1"/>
@@ -4104,7 +4176,7 @@
         <v>58</v>
       </c>
       <c r="R53" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S53" s="4">
         <f t="shared" si="1"/>
@@ -4164,7 +4236,7 @@
         <v>58</v>
       </c>
       <c r="R54" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S54" s="4">
         <f t="shared" si="1"/>
@@ -4224,7 +4296,7 @@
         <v>58</v>
       </c>
       <c r="R55" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S55" s="4">
         <f t="shared" si="1"/>
@@ -4284,7 +4356,7 @@
         <v>58</v>
       </c>
       <c r="R56" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S56" s="4">
         <f t="shared" si="1"/>
@@ -4344,7 +4416,7 @@
         <v>58</v>
       </c>
       <c r="R57" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S57" s="4">
         <f t="shared" si="1"/>
@@ -4404,7 +4476,7 @@
         <v>58</v>
       </c>
       <c r="R58" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S58" s="4">
         <f t="shared" si="1"/>
@@ -4464,7 +4536,7 @@
         <v>58</v>
       </c>
       <c r="R59" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S59" s="4">
         <f t="shared" si="1"/>
@@ -4473,7 +4545,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B60">
         <v>36</v>
@@ -4518,13 +4590,13 @@
         <v>0</v>
       </c>
       <c r="P60" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="Q60" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="R60" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S60" s="4">
         <f t="shared" si="1"/>
@@ -4533,7 +4605,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B61">
         <v>36</v>
@@ -4578,13 +4650,13 @@
         <v>0</v>
       </c>
       <c r="P61" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="Q61" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="R61" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S61" s="4">
         <f t="shared" si="1"/>
@@ -4593,13 +4665,13 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B62">
         <v>10</v>
       </c>
       <c r="C62">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4608,7 +4680,7 @@
         <v>1</v>
       </c>
       <c r="F62">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -4641,20 +4713,20 @@
         <v>83</v>
       </c>
       <c r="Q62" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R62" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S62" s="4">
         <f t="shared" si="1"/>
-        <v>279.095416661</v>
+        <v>312.09307094500002</v>
       </c>
       <c r="T62" s="4"/>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4669,7 +4741,7 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G63">
         <v>1</v>
@@ -4702,20 +4774,20 @@
         <v>83</v>
       </c>
       <c r="Q63" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="R63" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S63" s="4">
         <f t="shared" si="1"/>
-        <v>272.04834561400003</v>
+        <v>304.03817485799999</v>
       </c>
       <c r="T63" s="4"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B64">
         <v>10</v>
@@ -4763,10 +4835,10 @@
         <v>83</v>
       </c>
       <c r="Q64" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="R64" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="S64" s="4">
         <f t="shared" si="1"/>
@@ -4776,7 +4848,7 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B65">
         <v>45</v>
@@ -4821,13 +4893,13 @@
         <v>0</v>
       </c>
       <c r="P65" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Q65" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="R65" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S65" s="4">
         <f t="shared" si="1"/>
@@ -4837,7 +4909,7 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B66">
         <v>49</v>
@@ -4882,13 +4954,13 @@
         <v>0</v>
       </c>
       <c r="P66" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Q66" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="R66" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S66" s="4">
         <f t="shared" si="1"/>
@@ -4898,7 +4970,7 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B67">
         <v>47</v>
@@ -4943,13 +5015,13 @@
         <v>0</v>
       </c>
       <c r="P67" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="Q67" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="R67" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S67" s="4">
         <f t="shared" si="1"/>
@@ -4959,7 +5031,7 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B68">
         <v>46</v>
@@ -5004,13 +5076,13 @@
         <v>0</v>
       </c>
       <c r="P68" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="Q68" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R68" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S68" s="4">
         <f t="shared" si="1"/>
@@ -5020,7 +5092,7 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B69">
         <v>46</v>
@@ -5065,13 +5137,13 @@
         <v>0</v>
       </c>
       <c r="P69" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="Q69" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R69" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S69" s="4">
         <f t="shared" si="1"/>
@@ -5081,7 +5153,7 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B70">
         <v>40</v>
@@ -5126,13 +5198,13 @@
         <v>0</v>
       </c>
       <c r="P70" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Q70" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="R70" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S70" s="4">
         <f t="shared" si="1"/>
@@ -5142,7 +5214,7 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B71">
         <v>40</v>
@@ -5187,13 +5259,13 @@
         <v>0</v>
       </c>
       <c r="P71" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Q71" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="R71" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S71" s="4">
         <f t="shared" si="1"/>
@@ -5203,7 +5275,7 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B72">
         <v>45</v>
@@ -5248,13 +5320,13 @@
         <v>0</v>
       </c>
       <c r="P72" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q72" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R72" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S72" s="4">
         <f t="shared" si="1"/>
@@ -5264,7 +5336,7 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B73">
         <v>45</v>
@@ -5309,13 +5381,13 @@
         <v>0</v>
       </c>
       <c r="P73" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q73" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R73" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S73" s="4">
         <f t="shared" si="1"/>
@@ -5325,7 +5397,7 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B74">
         <v>44</v>
@@ -5370,13 +5442,13 @@
         <v>0</v>
       </c>
       <c r="P74" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q74" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R74" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S74" s="4">
         <f t="shared" si="1"/>
@@ -5386,7 +5458,7 @@
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B75">
         <v>44</v>
@@ -5431,13 +5503,13 @@
         <v>0</v>
       </c>
       <c r="P75" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q75" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R75" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S75" s="4">
         <f t="shared" si="1"/>
@@ -5447,7 +5519,7 @@
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B76">
         <v>43</v>
@@ -5492,13 +5564,13 @@
         <v>0</v>
       </c>
       <c r="P76" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q76" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R76" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S76" s="4">
         <f t="shared" si="1"/>
@@ -5508,7 +5580,7 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B77">
         <v>43</v>
@@ -5553,13 +5625,13 @@
         <v>0</v>
       </c>
       <c r="P77" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q77" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R77" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S77" s="4">
         <f t="shared" si="1"/>
@@ -5569,7 +5641,7 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B78">
         <v>42</v>
@@ -5614,13 +5686,13 @@
         <v>0</v>
       </c>
       <c r="P78" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q78" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R78" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S78" s="4">
         <f t="shared" si="1"/>
@@ -5630,7 +5702,7 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B79">
         <v>42</v>
@@ -5675,13 +5747,13 @@
         <v>0</v>
       </c>
       <c r="P79" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q79" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R79" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S79" s="4">
         <f t="shared" si="1"/>
@@ -5691,7 +5763,7 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B80">
         <v>41</v>
@@ -5736,13 +5808,13 @@
         <v>0</v>
       </c>
       <c r="P80" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q80" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R80" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S80" s="4">
         <f t="shared" si="1"/>
@@ -5752,7 +5824,7 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B81">
         <v>41</v>
@@ -5797,13 +5869,13 @@
         <v>0</v>
       </c>
       <c r="P81" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q81" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R81" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S81" s="4">
         <f t="shared" si="1"/>
@@ -5813,7 +5885,7 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B82">
         <v>40</v>
@@ -5858,13 +5930,13 @@
         <v>0</v>
       </c>
       <c r="P82" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q82" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R82" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S82" s="4">
         <f t="shared" ref="S82:S101" si="2">B82*$B$1+C82*$C$1+D82*$D$1+E82*$E$1+F82*$F$1+G82*$G$1+H82*$H$1+I82*$I$1+J82*$J$1+K82*$K$1+L82*$L$1+M82*$M$1+N82*$N$1+O82*$O$1</f>
@@ -5874,7 +5946,7 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B83">
         <v>40</v>
@@ -5919,13 +5991,13 @@
         <v>0</v>
       </c>
       <c r="P83" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q83" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R83" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S83" s="4">
         <f t="shared" si="2"/>
@@ -5935,7 +6007,7 @@
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B84">
         <v>39</v>
@@ -5980,13 +6052,13 @@
         <v>0</v>
       </c>
       <c r="P84" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q84" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R84" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S84" s="4">
         <f t="shared" si="2"/>
@@ -5996,7 +6068,7 @@
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B85">
         <v>39</v>
@@ -6041,13 +6113,13 @@
         <v>0</v>
       </c>
       <c r="P85" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q85" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R85" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S85" s="4">
         <f t="shared" si="2"/>
@@ -6057,7 +6129,7 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B86">
         <v>53</v>
@@ -6102,13 +6174,13 @@
         <v>0</v>
       </c>
       <c r="P86" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q86" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="R86" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S86" s="4">
         <f t="shared" si="2"/>
@@ -6118,7 +6190,7 @@
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B87">
         <v>53</v>
@@ -6163,13 +6235,13 @@
         <v>0</v>
       </c>
       <c r="P87" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q87" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="R87" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S87" s="4">
         <f t="shared" si="2"/>
@@ -6179,7 +6251,7 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B88">
         <v>53</v>
@@ -6224,13 +6296,13 @@
         <v>0</v>
       </c>
       <c r="P88" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q88" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R88" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S88" s="4">
         <f t="shared" si="2"/>
@@ -6240,7 +6312,7 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B89">
         <v>14</v>
@@ -6285,13 +6357,13 @@
         <v>0</v>
       </c>
       <c r="P89" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q89" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R89" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S89" s="4">
         <f t="shared" si="2"/>
@@ -6301,7 +6373,7 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B90">
         <v>19</v>
@@ -6346,13 +6418,13 @@
         <v>0</v>
       </c>
       <c r="P90" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q90" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R90" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S90" s="4">
         <f t="shared" si="2"/>
@@ -6362,7 +6434,7 @@
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B91">
         <v>24</v>
@@ -6407,13 +6479,13 @@
         <v>0</v>
       </c>
       <c r="P91" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q91" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R91" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S91" s="4">
         <f t="shared" si="2"/>
@@ -6423,7 +6495,7 @@
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B92">
         <v>29</v>
@@ -6468,13 +6540,13 @@
         <v>0</v>
       </c>
       <c r="P92" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q92" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R92" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S92" s="4">
         <f t="shared" si="2"/>
@@ -6484,7 +6556,7 @@
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B93">
         <v>34</v>
@@ -6529,13 +6601,13 @@
         <v>0</v>
       </c>
       <c r="P93" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q93" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R93" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S93" s="4">
         <f t="shared" si="2"/>
@@ -6545,7 +6617,7 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B94">
         <v>39</v>
@@ -6590,13 +6662,13 @@
         <v>0</v>
       </c>
       <c r="P94" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q94" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R94" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S94" s="4">
         <f t="shared" si="2"/>
@@ -6606,7 +6678,7 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B95">
         <v>44</v>
@@ -6651,13 +6723,13 @@
         <v>0</v>
       </c>
       <c r="P95" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q95" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R95" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S95" s="4">
         <f t="shared" si="2"/>
@@ -6667,7 +6739,7 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B96">
         <v>49</v>
@@ -6712,13 +6784,13 @@
         <v>0</v>
       </c>
       <c r="P96" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q96" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R96" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S96" s="4">
         <f t="shared" si="2"/>
@@ -6728,7 +6800,7 @@
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B97">
         <v>54</v>
@@ -6773,13 +6845,13 @@
         <v>0</v>
       </c>
       <c r="P97" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q97" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R97" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S97" s="4">
         <f t="shared" si="2"/>
@@ -6789,7 +6861,7 @@
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B98">
         <v>59</v>
@@ -6834,13 +6906,13 @@
         <v>0</v>
       </c>
       <c r="P98" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q98" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R98" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S98" s="4">
         <f t="shared" si="2"/>
@@ -6850,7 +6922,7 @@
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B99">
         <v>64</v>
@@ -6895,13 +6967,13 @@
         <v>0</v>
       </c>
       <c r="P99" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q99" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R99" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S99" s="4">
         <f t="shared" si="2"/>
@@ -6911,7 +6983,7 @@
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B100">
         <v>69</v>
@@ -6956,13 +7028,13 @@
         <v>0</v>
       </c>
       <c r="P100" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q100" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R100" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S100" s="4">
         <f t="shared" si="2"/>
@@ -6972,7 +7044,7 @@
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B101">
         <v>74</v>
@@ -7017,13 +7089,13 @@
         <v>0</v>
       </c>
       <c r="P101" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q101" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R101" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="S101" s="4">
         <f t="shared" si="2"/>
@@ -7041,8 +7113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q100"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7095,13 +7167,13 @@
         <v>44</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Q1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R1" t="s">
-        <v>95</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -7157,7 +7229,7 @@
         <v>53</v>
       </c>
       <c r="R2" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -7213,7 +7285,7 @@
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -7269,7 +7341,7 @@
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -7325,7 +7397,7 @@
         <v>2</v>
       </c>
       <c r="R5" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -7381,7 +7453,7 @@
         <v>3</v>
       </c>
       <c r="R6" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -7437,7 +7509,7 @@
         <v>4</v>
       </c>
       <c r="R7" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -7493,7 +7565,7 @@
         <v>5</v>
       </c>
       <c r="R8" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -7549,7 +7621,7 @@
         <v>6</v>
       </c>
       <c r="R9" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -7605,7 +7677,7 @@
         <v>92</v>
       </c>
       <c r="R10" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -7661,7 +7733,7 @@
         <v>7</v>
       </c>
       <c r="R11" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -7717,7 +7789,7 @@
         <v>8</v>
       </c>
       <c r="R12" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -7773,7 +7845,7 @@
         <v>58</v>
       </c>
       <c r="R13" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -7829,7 +7901,7 @@
         <v>9</v>
       </c>
       <c r="R14" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -7879,7 +7951,10 @@
         <v>0</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
+      </c>
+      <c r="R15" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -7929,10 +8004,13 @@
         <v>0</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="R16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -7979,10 +8057,13 @@
         <v>0</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -8029,10 +8110,13 @@
         <v>0</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -8079,10 +8163,13 @@
         <v>0</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -8129,10 +8216,13 @@
         <v>0</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -8179,10 +8269,13 @@
         <v>0</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
@@ -8229,10 +8322,13 @@
         <v>0</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -8279,10 +8375,13 @@
         <v>0</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -8329,10 +8428,13 @@
         <v>0</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -8379,10 +8481,13 @@
         <v>0</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -8429,10 +8534,13 @@
         <v>0</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -8479,10 +8587,13 @@
         <v>0</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="R27" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
@@ -8529,10 +8640,13 @@
         <v>0</v>
       </c>
       <c r="P28" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="R28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>22</v>
       </c>
@@ -8579,10 +8693,13 @@
         <v>0</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="R29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
@@ -8629,10 +8746,13 @@
         <v>0</v>
       </c>
       <c r="P30" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="R30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>24</v>
       </c>
@@ -8679,10 +8799,13 @@
         <v>0</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="R31" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>25</v>
       </c>
@@ -8729,7 +8852,10 @@
         <v>0</v>
       </c>
       <c r="P32" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R32" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -8779,7 +8905,10 @@
         <v>0</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R33" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
@@ -8829,7 +8958,10 @@
         <v>0</v>
       </c>
       <c r="P34" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R34" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
@@ -8879,7 +9011,10 @@
         <v>0</v>
       </c>
       <c r="P35" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R35" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
@@ -8929,7 +9064,10 @@
         <v>0</v>
       </c>
       <c r="P36" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="R36" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
@@ -8985,7 +9123,7 @@
         <v>20</v>
       </c>
       <c r="R37" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -9041,7 +9179,7 @@
         <v>58</v>
       </c>
       <c r="R38" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
@@ -9097,7 +9235,7 @@
         <v>58</v>
       </c>
       <c r="R39" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
@@ -9153,7 +9291,7 @@
         <v>58</v>
       </c>
       <c r="R40" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
@@ -9209,7 +9347,7 @@
         <v>58</v>
       </c>
       <c r="R41" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
@@ -9265,7 +9403,7 @@
         <v>58</v>
       </c>
       <c r="R42" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
@@ -9321,7 +9459,7 @@
         <v>58</v>
       </c>
       <c r="R43" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -9377,7 +9515,7 @@
         <v>58</v>
       </c>
       <c r="R44" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
@@ -9433,7 +9571,7 @@
         <v>58</v>
       </c>
       <c r="R45" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
@@ -9489,7 +9627,7 @@
         <v>58</v>
       </c>
       <c r="R46" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
@@ -9545,7 +9683,7 @@
         <v>58</v>
       </c>
       <c r="R47" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
@@ -9601,7 +9739,7 @@
         <v>58</v>
       </c>
       <c r="R48" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
@@ -9657,7 +9795,7 @@
         <v>58</v>
       </c>
       <c r="R49" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
@@ -9713,7 +9851,7 @@
         <v>58</v>
       </c>
       <c r="R50" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
@@ -9769,7 +9907,7 @@
         <v>58</v>
       </c>
       <c r="R51" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
@@ -9825,7 +9963,7 @@
         <v>58</v>
       </c>
       <c r="R52" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
@@ -9881,7 +10019,7 @@
         <v>58</v>
       </c>
       <c r="R53" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
@@ -9937,7 +10075,7 @@
         <v>58</v>
       </c>
       <c r="R54" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
@@ -9993,7 +10131,7 @@
         <v>58</v>
       </c>
       <c r="R55" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
@@ -10049,7 +10187,7 @@
         <v>58</v>
       </c>
       <c r="R56" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
@@ -10105,7 +10243,7 @@
         <v>58</v>
       </c>
       <c r="R57" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
@@ -10161,12 +10299,12 @@
         <v>58</v>
       </c>
       <c r="R58" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B59">
         <v>36</v>
@@ -10211,18 +10349,18 @@
         <v>0</v>
       </c>
       <c r="P59" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="Q59" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="R59" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B60">
         <v>36</v>
@@ -10267,24 +10405,24 @@
         <v>0</v>
       </c>
       <c r="P60" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="Q60" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="R60" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B61">
         <v>10</v>
       </c>
       <c r="C61">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -10293,7 +10431,7 @@
         <v>1</v>
       </c>
       <c r="F61">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -10326,15 +10464,15 @@
         <v>83</v>
       </c>
       <c r="Q61" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R61" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -10349,7 +10487,7 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -10382,15 +10520,15 @@
         <v>83</v>
       </c>
       <c r="Q62" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="R62" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B63">
         <v>10</v>
@@ -10438,15 +10576,15 @@
         <v>83</v>
       </c>
       <c r="Q63" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="R63" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B64">
         <v>45</v>
@@ -10491,18 +10629,18 @@
         <v>0</v>
       </c>
       <c r="P64" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Q64" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="R64" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B65">
         <v>49</v>
@@ -10547,18 +10685,18 @@
         <v>0</v>
       </c>
       <c r="P65" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Q65" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="R65" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B66">
         <v>47</v>
@@ -10603,18 +10741,18 @@
         <v>0</v>
       </c>
       <c r="P66" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="Q66" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="R66" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B67">
         <v>46</v>
@@ -10659,18 +10797,18 @@
         <v>0</v>
       </c>
       <c r="P67" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="Q67" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R67" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B68">
         <v>46</v>
@@ -10715,18 +10853,18 @@
         <v>0</v>
       </c>
       <c r="P68" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="Q68" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R68" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B69">
         <v>40</v>
@@ -10771,18 +10909,18 @@
         <v>0</v>
       </c>
       <c r="P69" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Q69" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="R69" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B70">
         <v>40</v>
@@ -10827,18 +10965,18 @@
         <v>0</v>
       </c>
       <c r="P70" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Q70" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="R70" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B71">
         <v>45</v>
@@ -10883,18 +11021,18 @@
         <v>0</v>
       </c>
       <c r="P71" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q71" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R71" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B72">
         <v>45</v>
@@ -10939,18 +11077,18 @@
         <v>0</v>
       </c>
       <c r="P72" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q72" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R72" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B73">
         <v>44</v>
@@ -10995,18 +11133,18 @@
         <v>0</v>
       </c>
       <c r="P73" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q73" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R73" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B74">
         <v>44</v>
@@ -11051,18 +11189,18 @@
         <v>0</v>
       </c>
       <c r="P74" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q74" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R74" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B75">
         <v>43</v>
@@ -11107,18 +11245,18 @@
         <v>0</v>
       </c>
       <c r="P75" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q75" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R75" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B76">
         <v>43</v>
@@ -11163,18 +11301,18 @@
         <v>0</v>
       </c>
       <c r="P76" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q76" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R76" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B77">
         <v>42</v>
@@ -11219,18 +11357,18 @@
         <v>0</v>
       </c>
       <c r="P77" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q77" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R77" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B78">
         <v>42</v>
@@ -11275,18 +11413,18 @@
         <v>0</v>
       </c>
       <c r="P78" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q78" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R78" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B79">
         <v>41</v>
@@ -11331,18 +11469,18 @@
         <v>0</v>
       </c>
       <c r="P79" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q79" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R79" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B80">
         <v>41</v>
@@ -11387,18 +11525,18 @@
         <v>0</v>
       </c>
       <c r="P80" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q80" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R80" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B81">
         <v>40</v>
@@ -11443,18 +11581,18 @@
         <v>0</v>
       </c>
       <c r="P81" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q81" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R81" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B82">
         <v>40</v>
@@ -11499,18 +11637,18 @@
         <v>0</v>
       </c>
       <c r="P82" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q82" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R82" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B83">
         <v>39</v>
@@ -11555,18 +11693,18 @@
         <v>0</v>
       </c>
       <c r="P83" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q83" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R83" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B84">
         <v>39</v>
@@ -11611,18 +11749,18 @@
         <v>0</v>
       </c>
       <c r="P84" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q84" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="R84" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B85">
         <v>53</v>
@@ -11667,18 +11805,18 @@
         <v>0</v>
       </c>
       <c r="P85" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q85" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="R85" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B86">
         <v>53</v>
@@ -11723,18 +11861,18 @@
         <v>0</v>
       </c>
       <c r="P86" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q86" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="R86" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B87">
         <v>53</v>
@@ -11779,18 +11917,18 @@
         <v>0</v>
       </c>
       <c r="P87" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q87" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R87" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B88">
         <v>14</v>
@@ -11835,18 +11973,18 @@
         <v>0</v>
       </c>
       <c r="P88" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q88" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R88" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B89">
         <v>19</v>
@@ -11891,18 +12029,18 @@
         <v>0</v>
       </c>
       <c r="P89" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q89" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R89" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B90">
         <v>24</v>
@@ -11947,18 +12085,18 @@
         <v>0</v>
       </c>
       <c r="P90" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q90" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R90" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B91">
         <v>29</v>
@@ -12003,18 +12141,18 @@
         <v>0</v>
       </c>
       <c r="P91" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q91" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R91" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B92">
         <v>34</v>
@@ -12059,18 +12197,18 @@
         <v>0</v>
       </c>
       <c r="P92" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q92" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R92" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B93">
         <v>39</v>
@@ -12115,18 +12253,18 @@
         <v>0</v>
       </c>
       <c r="P93" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q93" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R93" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B94">
         <v>44</v>
@@ -12171,18 +12309,18 @@
         <v>0</v>
       </c>
       <c r="P94" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q94" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R94" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B95">
         <v>49</v>
@@ -12227,18 +12365,18 @@
         <v>0</v>
       </c>
       <c r="P95" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q95" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R95" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B96">
         <v>54</v>
@@ -12283,18 +12421,18 @@
         <v>0</v>
       </c>
       <c r="P96" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q96" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R96" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B97">
         <v>59</v>
@@ -12339,18 +12477,18 @@
         <v>0</v>
       </c>
       <c r="P97" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q97" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R97" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B98">
         <v>64</v>
@@ -12395,18 +12533,18 @@
         <v>0</v>
       </c>
       <c r="P98" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q98" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R98" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B99">
         <v>69</v>
@@ -12451,18 +12589,18 @@
         <v>0</v>
       </c>
       <c r="P99" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q99" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R99" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B100">
         <v>74</v>
@@ -12507,13 +12645,13 @@
         <v>0</v>
       </c>
       <c r="P100" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q100" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="R100" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -12627,10 +12765,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12661,7 +12799,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -12686,7 +12824,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -12754,7 +12892,7 @@
         <v>42344</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
@@ -12787,10 +12925,10 @@
         <v>42624</v>
       </c>
       <c r="B23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -12798,10 +12936,10 @@
         <v>42709</v>
       </c>
       <c r="B24" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -12809,10 +12947,10 @@
         <v>42719</v>
       </c>
       <c r="B25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -12820,7 +12958,7 @@
         <v>42758</v>
       </c>
       <c r="B26" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C26" t="s">
         <v>50</v>
@@ -12831,7 +12969,7 @@
         <v>42758</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C27" t="s">
         <v>50</v>
@@ -12842,7 +12980,7 @@
         <v>42758</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C28" t="s">
         <v>50</v>
@@ -12853,7 +12991,7 @@
         <v>42758</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
@@ -12864,9 +13002,31 @@
         <v>42758</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>42759</v>
+      </c>
+      <c r="B31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>42759</v>
+      </c>
+      <c r="B32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finally fixing definitions for PDPT, S_DGCC base fragments
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_basic_component_matrix.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_basic_component_matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="460" windowWidth="25040" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="1640" yWindow="460" windowWidth="25040" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Elemental composition matrix" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="170">
   <si>
     <t>DGCC</t>
   </si>
@@ -533,7 +533,13 @@
     <t>DB_unique_species</t>
   </si>
   <si>
-    <t>Fixed composition definitions of BLL, PDPT (still verifying PDPT &amp; waiting on verification for S_DGCC)</t>
+    <t>Fixed composition definitions of BLL (still verifying PDPT &amp; waiting on verification for S_DGCC)</t>
+  </si>
+  <si>
+    <t>Fixed composition definitions of PDPT and S_DGCC</t>
+  </si>
+  <si>
+    <t>HFF</t>
   </si>
 </sst>
 </file>
@@ -1071,10 +1077,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane ySplit="1080" topLeftCell="A52" activePane="bottomLeft"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <pane ySplit="1080" activePane="bottomLeft"/>
       <selection activeCell="R3" sqref="R3"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:R101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4671,7 +4677,7 @@
         <v>10</v>
       </c>
       <c r="C62">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4720,7 +4726,7 @@
       </c>
       <c r="S62" s="4">
         <f t="shared" si="1"/>
-        <v>312.09307094500002</v>
+        <v>311.08524590499997</v>
       </c>
       <c r="T62" s="4"/>
     </row>
@@ -4802,7 +4808,7 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -4842,7 +4848,7 @@
       </c>
       <c r="S64" s="4">
         <f t="shared" si="1"/>
-        <v>266.08240914200002</v>
+        <v>298.07223838599998</v>
       </c>
       <c r="T64" s="4"/>
     </row>
@@ -7113,8 +7119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10422,7 +10428,7 @@
         <v>10</v>
       </c>
       <c r="C61">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -10543,7 +10549,7 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -12765,10 +12771,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13030,6 +13036,17 @@
         <v>50</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>42760</v>
+      </c>
+      <c r="B33" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Some additional notes on the notes tab of master component matrix spreadsheet
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_basic_component_matrix.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_basic_component_matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="460" windowWidth="25040" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1640" yWindow="460" windowWidth="25040" windowHeight="17460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Elemental composition matrix" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="172">
   <si>
     <t>DGCC</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Matrix created and validated</t>
   </si>
   <si>
-    <t>Navigate to second tab, "For export to .csv"</t>
-  </si>
-  <si>
     <t>FFA</t>
   </si>
   <si>
@@ -290,9 +287,6 @@
     <t>Latest versions of all pipeline scripts and required files available at https://github.com/vanmooylipidomics/LOBSTAHS, or upon demand from Dr. Fredricks</t>
   </si>
   <si>
-    <t>If making any additions or modifications to the default set of entires, do these in the worksheet on the first tab; then, paste any of the additional/modified entries "as values" into the third tab before saving</t>
-  </si>
-  <si>
     <t>Updated some comments</t>
   </si>
   <si>
@@ -302,9 +296,6 @@
     <t>Can be used to generate "LOBSTAHS_basic_component_matrix.csv," required for lipid-oxlipid-oxyipin database generation in the LOBSTAHS lipidomics screening pipeline</t>
   </si>
   <si>
-    <t>Export the worksheet as a .csv file with the filename "LOBSTAHS_basic_component_matrix.csv"; this file can be sourced by specifying the file path in the LOBSTAHS database generation function</t>
-  </si>
-  <si>
     <t>Fixed error in DNPPE components</t>
   </si>
   <si>
@@ -540,6 +531,21 @@
   </si>
   <si>
     <t>HFF</t>
+  </si>
+  <si>
+    <t>When done with edits/additions, copy all data in "Elemental composition matrix" except for the first row and last column</t>
+  </si>
+  <si>
+    <t>Navigate to second tab, "For export to .csv," then paste the data copied from the first worksheet "as values"</t>
+  </si>
+  <si>
+    <t>Make any additions or modifications to the default set of entries by editing data in the first worksheet ("Elemental composition matrix")</t>
+  </si>
+  <si>
+    <t>Export the "For export to .csv" worksheet as a .csv file with the filename "LOBSTAHS_basic_component_matrix.csv"; this file can be sourced by specifying the file path in the LOBSTAHS database generation function</t>
+  </si>
+  <si>
+    <t>Note any changes in changelog (this "Notes" worksheet); consider requesting incorporation of your new lipids into the default LOBSTAHS database via a pull request on GitHub</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1086,7 @@
     <sheetView topLeftCell="A2" workbookViewId="0">
       <pane ySplit="1080" activePane="bottomLeft"/>
       <selection activeCell="R3" sqref="R3"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:R101"/>
+      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1147,7 +1153,7 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
@@ -1171,25 +1177,25 @@
         <v>38</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M2" t="s">
         <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O2" t="s">
         <v>44</v>
       </c>
       <c r="P2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="R2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="S2" t="s">
         <v>43</v>
@@ -1197,7 +1203,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1242,13 +1248,13 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" ref="S3:S15" si="0">B3*$B$1+C3*$C$1+D3*$D$1+E3*$E$1+F3*$F$1+G3*$G$1+H3*$H$1+I3*$I$1+J3*$J$1+K3*$K$1+L3*$L$1+M3*$M$1+N3*$N$1+O3*$O$1</f>
@@ -1302,13 +1308,13 @@
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q4" t="s">
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="0"/>
@@ -1362,13 +1368,13 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q5" t="s">
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S5" s="4">
         <f t="shared" si="0"/>
@@ -1422,13 +1428,13 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q6" t="s">
         <v>2</v>
       </c>
       <c r="R6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S6" s="4">
         <f t="shared" si="0"/>
@@ -1488,7 +1494,7 @@
         <v>3</v>
       </c>
       <c r="R7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S7" s="4">
         <f t="shared" si="0"/>
@@ -1542,13 +1548,13 @@
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q8" t="s">
         <v>4</v>
       </c>
       <c r="R8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" si="0"/>
@@ -1602,13 +1608,13 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q9" t="s">
         <v>5</v>
       </c>
       <c r="R9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S9" s="4">
         <f t="shared" si="0"/>
@@ -1662,13 +1668,13 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q10" t="s">
         <v>6</v>
       </c>
       <c r="R10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S10" s="4">
         <f t="shared" si="0"/>
@@ -1677,7 +1683,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -1722,13 +1728,13 @@
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S11" s="4">
         <f t="shared" si="0"/>
@@ -1788,7 +1794,7 @@
         <v>7</v>
       </c>
       <c r="R12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S12" s="4">
         <f t="shared" si="0"/>
@@ -1842,13 +1848,13 @@
         <v>0</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q13" s="7" t="s">
         <v>8</v>
       </c>
       <c r="R13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S13" s="4">
         <f t="shared" si="0"/>
@@ -1857,7 +1863,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14">
         <v>55</v>
@@ -1902,13 +1908,13 @@
         <v>1</v>
       </c>
       <c r="P14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S14" s="4">
         <f t="shared" si="0"/>
@@ -1962,13 +1968,13 @@
         <v>0</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="R15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S15" s="4">
         <f t="shared" si="0"/>
@@ -2022,10 +2028,10 @@
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="R16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="S16" s="4">
         <f>B16*$B$1+C16*$C$1+D16*$D$1+E16*$E$1+F16*$F$1+G16*$G$1+H16*$H$1+I16*$I$1+J16*$J$1+K16*$K$1+L16*$L$1</f>
@@ -2079,10 +2085,10 @@
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="R17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="S17" s="4">
         <f>B17*$B$1+C17*$C$1+D17*$D$1+E17*$E$1+F17*$F$1+G17*$G$1+H17*$H$1+I17*$I$1+J17*$J$1+K17*$K$1+L17*$L$1</f>
@@ -2136,10 +2142,10 @@
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S18" s="4">
         <f t="shared" ref="S18:S81" si="1">B18*$B$1+C18*$C$1+D18*$D$1+E18*$E$1+F18*$F$1+G18*$G$1+H18*$H$1+I18*$I$1+J18*$J$1+K18*$K$1+L18*$L$1+M18*$M$1+N18*$N$1+O18*$O$1</f>
@@ -2193,10 +2199,10 @@
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S19" s="4">
         <f t="shared" si="1"/>
@@ -2250,10 +2256,10 @@
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S20" s="4">
         <f t="shared" si="1"/>
@@ -2307,10 +2313,10 @@
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S21" s="4">
         <f t="shared" si="1"/>
@@ -2364,10 +2370,10 @@
         <v>0</v>
       </c>
       <c r="P22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S22" s="4">
         <f t="shared" si="1"/>
@@ -2376,7 +2382,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -2421,10 +2427,10 @@
         <v>0</v>
       </c>
       <c r="P23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S23" s="4">
         <f t="shared" si="1"/>
@@ -2478,10 +2484,10 @@
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S24" s="4">
         <f t="shared" si="1"/>
@@ -2535,10 +2541,10 @@
         <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="1"/>
@@ -2592,10 +2598,10 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S26" s="4">
         <f t="shared" si="1"/>
@@ -2649,10 +2655,10 @@
         <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S27" s="4">
         <f t="shared" si="1"/>
@@ -2706,10 +2712,10 @@
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="S28" s="4">
         <f t="shared" si="1"/>
@@ -2763,10 +2769,10 @@
         <v>0</v>
       </c>
       <c r="P29" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R29" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S29" s="4">
         <f t="shared" si="1"/>
@@ -2820,10 +2826,10 @@
         <v>0</v>
       </c>
       <c r="P30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S30" s="4">
         <f t="shared" si="1"/>
@@ -2877,10 +2883,10 @@
         <v>0</v>
       </c>
       <c r="P31" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R31" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S31" s="4">
         <f t="shared" si="1"/>
@@ -2934,10 +2940,10 @@
         <v>0</v>
       </c>
       <c r="P32" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R32" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S32" s="4">
         <f t="shared" si="1"/>
@@ -2991,10 +2997,10 @@
         <v>0</v>
       </c>
       <c r="P33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S33" s="4">
         <f t="shared" si="1"/>
@@ -3048,10 +3054,10 @@
         <v>0</v>
       </c>
       <c r="P34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S34" s="4">
         <f t="shared" si="1"/>
@@ -3105,10 +3111,10 @@
         <v>0</v>
       </c>
       <c r="P35" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R35" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S35" s="4">
         <f t="shared" si="1"/>
@@ -3162,10 +3168,10 @@
         <v>0</v>
       </c>
       <c r="P36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S36" s="4">
         <f t="shared" si="1"/>
@@ -3219,10 +3225,10 @@
         <v>0</v>
       </c>
       <c r="P37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S37" s="4">
         <f t="shared" si="1"/>
@@ -3282,7 +3288,7 @@
         <v>20</v>
       </c>
       <c r="R38" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S38" s="4">
         <f t="shared" si="1"/>
@@ -3291,7 +3297,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39">
         <v>46</v>
@@ -3336,13 +3342,13 @@
         <v>0</v>
       </c>
       <c r="P39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R39" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S39" s="4">
         <f t="shared" si="1"/>
@@ -3351,7 +3357,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40">
         <v>48</v>
@@ -3396,13 +3402,13 @@
         <v>0</v>
       </c>
       <c r="P40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R40" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S40" s="4">
         <f t="shared" si="1"/>
@@ -3411,7 +3417,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -3456,13 +3462,13 @@
         <v>0</v>
       </c>
       <c r="P41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S41" s="4">
         <f t="shared" si="1"/>
@@ -3471,7 +3477,7 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42">
         <v>40</v>
@@ -3516,13 +3522,13 @@
         <v>0</v>
       </c>
       <c r="P42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R42" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S42" s="4">
         <f t="shared" si="1"/>
@@ -3531,7 +3537,7 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43">
         <v>40</v>
@@ -3576,13 +3582,13 @@
         <v>0</v>
       </c>
       <c r="P43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S43" s="4">
         <f t="shared" si="1"/>
@@ -3591,7 +3597,7 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44">
         <v>55</v>
@@ -3636,13 +3642,13 @@
         <v>1</v>
       </c>
       <c r="P44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R44" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S44" s="4">
         <f t="shared" si="1"/>
@@ -3651,7 +3657,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45">
         <v>35</v>
@@ -3696,13 +3702,13 @@
         <v>1</v>
       </c>
       <c r="P45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R45" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S45" s="4">
         <f t="shared" si="1"/>
@@ -3711,7 +3717,7 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B46">
         <v>36</v>
@@ -3756,13 +3762,13 @@
         <v>1</v>
       </c>
       <c r="P46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R46" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S46" s="4">
         <f t="shared" si="1"/>
@@ -3771,7 +3777,7 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B47">
         <v>35</v>
@@ -3816,13 +3822,13 @@
         <v>1</v>
       </c>
       <c r="P47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R47" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S47" s="4">
         <f t="shared" si="1"/>
@@ -3831,7 +3837,7 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B48">
         <v>40</v>
@@ -3876,13 +3882,13 @@
         <v>0</v>
       </c>
       <c r="P48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R48" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S48" s="4">
         <f t="shared" si="1"/>
@@ -3891,7 +3897,7 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B49">
         <v>40</v>
@@ -3936,13 +3942,13 @@
         <v>0</v>
       </c>
       <c r="P49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R49" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S49" s="4">
         <f t="shared" si="1"/>
@@ -3951,7 +3957,7 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50">
         <v>40</v>
@@ -3996,13 +4002,13 @@
         <v>0</v>
       </c>
       <c r="P50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R50" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S50" s="4">
         <f t="shared" si="1"/>
@@ -4011,7 +4017,7 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51">
         <v>40</v>
@@ -4056,13 +4062,13 @@
         <v>0</v>
       </c>
       <c r="P51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R51" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S51" s="4">
         <f t="shared" si="1"/>
@@ -4071,7 +4077,7 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B52">
         <v>42</v>
@@ -4116,13 +4122,13 @@
         <v>0</v>
       </c>
       <c r="P52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R52" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S52" s="4">
         <f t="shared" si="1"/>
@@ -4131,7 +4137,7 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B53">
         <v>40</v>
@@ -4176,13 +4182,13 @@
         <v>0</v>
       </c>
       <c r="P53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R53" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S53" s="4">
         <f t="shared" si="1"/>
@@ -4191,7 +4197,7 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B54">
         <v>40</v>
@@ -4236,13 +4242,13 @@
         <v>0</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R54" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S54" s="4">
         <f t="shared" si="1"/>
@@ -4251,7 +4257,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55">
         <v>39</v>
@@ -4296,13 +4302,13 @@
         <v>0</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R55" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S55" s="4">
         <f t="shared" si="1"/>
@@ -4311,7 +4317,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56">
         <v>55</v>
@@ -4356,13 +4362,13 @@
         <v>0</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R56" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S56" s="4">
         <f t="shared" si="1"/>
@@ -4371,7 +4377,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B57">
         <v>40</v>
@@ -4416,13 +4422,13 @@
         <v>0</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R57" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S57" s="4">
         <f t="shared" si="1"/>
@@ -4431,7 +4437,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58">
         <v>40</v>
@@ -4476,13 +4482,13 @@
         <v>0</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R58" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S58" s="4">
         <f t="shared" si="1"/>
@@ -4491,7 +4497,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59">
         <v>40</v>
@@ -4536,13 +4542,13 @@
         <v>0</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R59" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S59" s="4">
         <f t="shared" si="1"/>
@@ -4551,7 +4557,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B60">
         <v>36</v>
@@ -4596,13 +4602,13 @@
         <v>0</v>
       </c>
       <c r="P60" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="Q60" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="R60" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S60" s="4">
         <f t="shared" si="1"/>
@@ -4611,7 +4617,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B61">
         <v>36</v>
@@ -4656,13 +4662,13 @@
         <v>0</v>
       </c>
       <c r="P61" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="Q61" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="R61" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S61" s="4">
         <f t="shared" si="1"/>
@@ -4671,7 +4677,7 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B62">
         <v>10</v>
@@ -4716,13 +4722,13 @@
         <v>0</v>
       </c>
       <c r="P62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q62" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="R62" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S62" s="4">
         <f t="shared" si="1"/>
@@ -4732,7 +4738,7 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4777,13 +4783,13 @@
         <v>0</v>
       </c>
       <c r="P63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q63" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="R63" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S63" s="4">
         <f t="shared" si="1"/>
@@ -4793,7 +4799,7 @@
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B64">
         <v>10</v>
@@ -4838,13 +4844,13 @@
         <v>0</v>
       </c>
       <c r="P64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q64" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="R64" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S64" s="4">
         <f t="shared" si="1"/>
@@ -4854,7 +4860,7 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B65">
         <v>45</v>
@@ -4899,13 +4905,13 @@
         <v>0</v>
       </c>
       <c r="P65" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Q65" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="R65" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S65" s="4">
         <f t="shared" si="1"/>
@@ -4915,7 +4921,7 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B66">
         <v>49</v>
@@ -4960,13 +4966,13 @@
         <v>0</v>
       </c>
       <c r="P66" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="Q66" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R66" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S66" s="4">
         <f t="shared" si="1"/>
@@ -4976,7 +4982,7 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B67">
         <v>47</v>
@@ -5021,13 +5027,13 @@
         <v>0</v>
       </c>
       <c r="P67" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q67" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="R67" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S67" s="4">
         <f t="shared" si="1"/>
@@ -5037,7 +5043,7 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B68">
         <v>46</v>
@@ -5082,13 +5088,13 @@
         <v>0</v>
       </c>
       <c r="P68" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Q68" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="R68" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S68" s="4">
         <f t="shared" si="1"/>
@@ -5098,7 +5104,7 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B69">
         <v>46</v>
@@ -5143,13 +5149,13 @@
         <v>0</v>
       </c>
       <c r="P69" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Q69" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="R69" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S69" s="4">
         <f t="shared" si="1"/>
@@ -5159,7 +5165,7 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B70">
         <v>40</v>
@@ -5204,13 +5210,13 @@
         <v>0</v>
       </c>
       <c r="P70" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="Q70" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="R70" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S70" s="4">
         <f t="shared" si="1"/>
@@ -5220,7 +5226,7 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B71">
         <v>40</v>
@@ -5265,13 +5271,13 @@
         <v>0</v>
       </c>
       <c r="P71" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="Q71" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="R71" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S71" s="4">
         <f t="shared" si="1"/>
@@ -5281,7 +5287,7 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B72">
         <v>45</v>
@@ -5326,13 +5332,13 @@
         <v>0</v>
       </c>
       <c r="P72" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q72" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R72" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S72" s="4">
         <f t="shared" si="1"/>
@@ -5342,7 +5348,7 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B73">
         <v>45</v>
@@ -5387,13 +5393,13 @@
         <v>0</v>
       </c>
       <c r="P73" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q73" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R73" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S73" s="4">
         <f t="shared" si="1"/>
@@ -5403,7 +5409,7 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B74">
         <v>44</v>
@@ -5448,13 +5454,13 @@
         <v>0</v>
       </c>
       <c r="P74" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q74" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R74" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S74" s="4">
         <f t="shared" si="1"/>
@@ -5464,7 +5470,7 @@
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B75">
         <v>44</v>
@@ -5509,13 +5515,13 @@
         <v>0</v>
       </c>
       <c r="P75" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q75" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R75" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S75" s="4">
         <f t="shared" si="1"/>
@@ -5525,7 +5531,7 @@
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B76">
         <v>43</v>
@@ -5570,13 +5576,13 @@
         <v>0</v>
       </c>
       <c r="P76" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q76" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R76" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S76" s="4">
         <f t="shared" si="1"/>
@@ -5586,7 +5592,7 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B77">
         <v>43</v>
@@ -5631,13 +5637,13 @@
         <v>0</v>
       </c>
       <c r="P77" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q77" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R77" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S77" s="4">
         <f t="shared" si="1"/>
@@ -5647,7 +5653,7 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B78">
         <v>42</v>
@@ -5692,13 +5698,13 @@
         <v>0</v>
       </c>
       <c r="P78" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q78" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R78" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S78" s="4">
         <f t="shared" si="1"/>
@@ -5708,7 +5714,7 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B79">
         <v>42</v>
@@ -5753,13 +5759,13 @@
         <v>0</v>
       </c>
       <c r="P79" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q79" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R79" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S79" s="4">
         <f t="shared" si="1"/>
@@ -5769,7 +5775,7 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B80">
         <v>41</v>
@@ -5814,13 +5820,13 @@
         <v>0</v>
       </c>
       <c r="P80" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q80" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R80" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S80" s="4">
         <f t="shared" si="1"/>
@@ -5830,7 +5836,7 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B81">
         <v>41</v>
@@ -5875,13 +5881,13 @@
         <v>0</v>
       </c>
       <c r="P81" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q81" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R81" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S81" s="4">
         <f t="shared" si="1"/>
@@ -5891,7 +5897,7 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B82">
         <v>40</v>
@@ -5936,13 +5942,13 @@
         <v>0</v>
       </c>
       <c r="P82" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q82" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R82" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S82" s="4">
         <f t="shared" ref="S82:S101" si="2">B82*$B$1+C82*$C$1+D82*$D$1+E82*$E$1+F82*$F$1+G82*$G$1+H82*$H$1+I82*$I$1+J82*$J$1+K82*$K$1+L82*$L$1+M82*$M$1+N82*$N$1+O82*$O$1</f>
@@ -5952,7 +5958,7 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B83">
         <v>40</v>
@@ -5997,13 +6003,13 @@
         <v>0</v>
       </c>
       <c r="P83" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q83" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R83" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S83" s="4">
         <f t="shared" si="2"/>
@@ -6013,7 +6019,7 @@
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B84">
         <v>39</v>
@@ -6058,13 +6064,13 @@
         <v>0</v>
       </c>
       <c r="P84" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q84" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R84" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S84" s="4">
         <f t="shared" si="2"/>
@@ -6074,7 +6080,7 @@
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B85">
         <v>39</v>
@@ -6119,13 +6125,13 @@
         <v>0</v>
       </c>
       <c r="P85" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q85" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R85" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S85" s="4">
         <f t="shared" si="2"/>
@@ -6135,7 +6141,7 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B86">
         <v>53</v>
@@ -6180,13 +6186,13 @@
         <v>0</v>
       </c>
       <c r="P86" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="Q86" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="R86" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S86" s="4">
         <f t="shared" si="2"/>
@@ -6196,7 +6202,7 @@
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B87">
         <v>53</v>
@@ -6241,13 +6247,13 @@
         <v>0</v>
       </c>
       <c r="P87" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="Q87" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="R87" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S87" s="4">
         <f t="shared" si="2"/>
@@ -6257,7 +6263,7 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B88">
         <v>53</v>
@@ -6302,13 +6308,13 @@
         <v>0</v>
       </c>
       <c r="P88" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="Q88" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="R88" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S88" s="4">
         <f t="shared" si="2"/>
@@ -6318,7 +6324,7 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B89">
         <v>14</v>
@@ -6363,13 +6369,13 @@
         <v>0</v>
       </c>
       <c r="P89" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q89" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R89" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S89" s="4">
         <f t="shared" si="2"/>
@@ -6379,7 +6385,7 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B90">
         <v>19</v>
@@ -6424,13 +6430,13 @@
         <v>0</v>
       </c>
       <c r="P90" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q90" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R90" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S90" s="4">
         <f t="shared" si="2"/>
@@ -6440,7 +6446,7 @@
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B91">
         <v>24</v>
@@ -6485,13 +6491,13 @@
         <v>0</v>
       </c>
       <c r="P91" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q91" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R91" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S91" s="4">
         <f t="shared" si="2"/>
@@ -6501,7 +6507,7 @@
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B92">
         <v>29</v>
@@ -6546,13 +6552,13 @@
         <v>0</v>
       </c>
       <c r="P92" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q92" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R92" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S92" s="4">
         <f t="shared" si="2"/>
@@ -6562,7 +6568,7 @@
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B93">
         <v>34</v>
@@ -6607,13 +6613,13 @@
         <v>0</v>
       </c>
       <c r="P93" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q93" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R93" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S93" s="4">
         <f t="shared" si="2"/>
@@ -6623,7 +6629,7 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B94">
         <v>39</v>
@@ -6668,13 +6674,13 @@
         <v>0</v>
       </c>
       <c r="P94" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q94" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R94" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S94" s="4">
         <f t="shared" si="2"/>
@@ -6684,7 +6690,7 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B95">
         <v>44</v>
@@ -6729,13 +6735,13 @@
         <v>0</v>
       </c>
       <c r="P95" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q95" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R95" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S95" s="4">
         <f t="shared" si="2"/>
@@ -6745,7 +6751,7 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B96">
         <v>49</v>
@@ -6790,13 +6796,13 @@
         <v>0</v>
       </c>
       <c r="P96" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q96" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R96" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S96" s="4">
         <f t="shared" si="2"/>
@@ -6806,7 +6812,7 @@
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B97">
         <v>54</v>
@@ -6851,13 +6857,13 @@
         <v>0</v>
       </c>
       <c r="P97" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q97" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R97" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S97" s="4">
         <f t="shared" si="2"/>
@@ -6867,7 +6873,7 @@
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B98">
         <v>59</v>
@@ -6912,13 +6918,13 @@
         <v>0</v>
       </c>
       <c r="P98" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q98" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R98" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S98" s="4">
         <f t="shared" si="2"/>
@@ -6928,7 +6934,7 @@
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B99">
         <v>64</v>
@@ -6973,13 +6979,13 @@
         <v>0</v>
       </c>
       <c r="P99" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q99" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R99" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S99" s="4">
         <f t="shared" si="2"/>
@@ -6989,7 +6995,7 @@
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B100">
         <v>69</v>
@@ -7034,13 +7040,13 @@
         <v>0</v>
       </c>
       <c r="P100" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q100" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R100" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S100" s="4">
         <f t="shared" si="2"/>
@@ -7050,7 +7056,7 @@
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B101">
         <v>74</v>
@@ -7095,13 +7101,13 @@
         <v>0</v>
       </c>
       <c r="P101" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q101" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R101" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S101" s="4">
         <f t="shared" si="2"/>
@@ -7119,8 +7125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7137,7 +7143,7 @@
         <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
         <v>32</v>
@@ -7161,30 +7167,30 @@
         <v>38</v>
       </c>
       <c r="L1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M1" t="s">
         <v>42</v>
       </c>
       <c r="N1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O1" t="s">
         <v>44</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="R1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -7229,13 +7235,13 @@
         <v>0</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -7285,13 +7291,13 @@
         <v>0</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q3" t="s">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -7341,13 +7347,13 @@
         <v>0</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q4" t="s">
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -7397,13 +7403,13 @@
         <v>0</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q5" t="s">
         <v>2</v>
       </c>
       <c r="R5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -7459,7 +7465,7 @@
         <v>3</v>
       </c>
       <c r="R6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -7509,13 +7515,13 @@
         <v>0</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q7" t="s">
         <v>4</v>
       </c>
       <c r="R7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -7565,13 +7571,13 @@
         <v>0</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q8" t="s">
         <v>5</v>
       </c>
       <c r="R8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -7621,18 +7627,18 @@
         <v>0</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q9" t="s">
         <v>6</v>
       </c>
       <c r="R9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -7677,13 +7683,13 @@
         <v>0</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -7739,7 +7745,7 @@
         <v>7</v>
       </c>
       <c r="R11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -7789,18 +7795,18 @@
         <v>0</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="R12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13">
         <v>55</v>
@@ -7845,13 +7851,13 @@
         <v>1</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -7901,13 +7907,13 @@
         <v>0</v>
       </c>
       <c r="P14" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="R14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -7957,10 +7963,10 @@
         <v>0</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="R15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -8010,10 +8016,10 @@
         <v>0</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="R16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -8063,10 +8069,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -8116,10 +8122,10 @@
         <v>0</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -8169,10 +8175,10 @@
         <v>0</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -8222,10 +8228,10 @@
         <v>0</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -8275,15 +8281,15 @@
         <v>0</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -8328,10 +8334,10 @@
         <v>0</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -8381,10 +8387,10 @@
         <v>0</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
@@ -8434,10 +8440,10 @@
         <v>0</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
@@ -8487,10 +8493,10 @@
         <v>0</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
@@ -8540,10 +8546,10 @@
         <v>0</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
@@ -8593,10 +8599,10 @@
         <v>0</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -8646,10 +8652,10 @@
         <v>0</v>
       </c>
       <c r="P28" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
@@ -8699,10 +8705,10 @@
         <v>0</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R29" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
@@ -8752,10 +8758,10 @@
         <v>0</v>
       </c>
       <c r="P30" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
@@ -8805,10 +8811,10 @@
         <v>0</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R31" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
@@ -8858,10 +8864,10 @@
         <v>0</v>
       </c>
       <c r="P32" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R32" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -8911,10 +8917,10 @@
         <v>0</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
@@ -8964,10 +8970,10 @@
         <v>0</v>
       </c>
       <c r="P34" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
@@ -9017,10 +9023,10 @@
         <v>0</v>
       </c>
       <c r="P35" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R35" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
@@ -9070,10 +9076,10 @@
         <v>0</v>
       </c>
       <c r="P36" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="R36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
@@ -9129,12 +9135,12 @@
         <v>20</v>
       </c>
       <c r="R37" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38">
         <v>46</v>
@@ -9179,18 +9185,18 @@
         <v>0</v>
       </c>
       <c r="P38" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R38" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B39">
         <v>48</v>
@@ -9235,18 +9241,18 @@
         <v>0</v>
       </c>
       <c r="P39" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R39" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40">
         <v>40</v>
@@ -9291,18 +9297,18 @@
         <v>0</v>
       </c>
       <c r="P40" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R40" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -9347,18 +9353,18 @@
         <v>0</v>
       </c>
       <c r="P41" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B42">
         <v>40</v>
@@ -9403,18 +9409,18 @@
         <v>0</v>
       </c>
       <c r="P42" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R42" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B43">
         <v>55</v>
@@ -9459,18 +9465,18 @@
         <v>1</v>
       </c>
       <c r="P43" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B44">
         <v>35</v>
@@ -9515,18 +9521,18 @@
         <v>1</v>
       </c>
       <c r="P44" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R44" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B45">
         <v>36</v>
@@ -9571,18 +9577,18 @@
         <v>1</v>
       </c>
       <c r="P45" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R45" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46">
         <v>35</v>
@@ -9627,18 +9633,18 @@
         <v>1</v>
       </c>
       <c r="P46" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R46" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B47">
         <v>40</v>
@@ -9683,18 +9689,18 @@
         <v>0</v>
       </c>
       <c r="P47" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R47" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B48">
         <v>40</v>
@@ -9739,18 +9745,18 @@
         <v>0</v>
       </c>
       <c r="P48" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R48" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B49">
         <v>40</v>
@@ -9795,18 +9801,18 @@
         <v>0</v>
       </c>
       <c r="P49" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R49" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B50">
         <v>40</v>
@@ -9851,18 +9857,18 @@
         <v>0</v>
       </c>
       <c r="P50" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R50" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B51">
         <v>42</v>
@@ -9907,18 +9913,18 @@
         <v>0</v>
       </c>
       <c r="P51" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R51" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B52">
         <v>40</v>
@@ -9963,18 +9969,18 @@
         <v>0</v>
       </c>
       <c r="P52" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R52" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B53">
         <v>40</v>
@@ -10019,18 +10025,18 @@
         <v>0</v>
       </c>
       <c r="P53" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R53" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B54">
         <v>39</v>
@@ -10075,18 +10081,18 @@
         <v>0</v>
       </c>
       <c r="P54" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R54" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B55">
         <v>55</v>
@@ -10131,18 +10137,18 @@
         <v>0</v>
       </c>
       <c r="P55" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R55" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B56">
         <v>40</v>
@@ -10187,18 +10193,18 @@
         <v>0</v>
       </c>
       <c r="P56" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R56" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B57">
         <v>40</v>
@@ -10243,18 +10249,18 @@
         <v>0</v>
       </c>
       <c r="P57" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R57" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B58">
         <v>40</v>
@@ -10299,18 +10305,18 @@
         <v>0</v>
       </c>
       <c r="P58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R58" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B59">
         <v>36</v>
@@ -10355,18 +10361,18 @@
         <v>0</v>
       </c>
       <c r="P59" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="Q59" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="R59" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B60">
         <v>36</v>
@@ -10411,18 +10417,18 @@
         <v>0</v>
       </c>
       <c r="P60" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="Q60" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="R60" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B61">
         <v>10</v>
@@ -10467,18 +10473,18 @@
         <v>0</v>
       </c>
       <c r="P61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q61" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="R61" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -10523,18 +10529,18 @@
         <v>0</v>
       </c>
       <c r="P62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q62" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="R62" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B63">
         <v>10</v>
@@ -10579,18 +10585,18 @@
         <v>0</v>
       </c>
       <c r="P63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q63" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="R63" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B64">
         <v>45</v>
@@ -10635,18 +10641,18 @@
         <v>0</v>
       </c>
       <c r="P64" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Q64" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="R64" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B65">
         <v>49</v>
@@ -10691,18 +10697,18 @@
         <v>0</v>
       </c>
       <c r="P65" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="Q65" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R65" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B66">
         <v>47</v>
@@ -10747,18 +10753,18 @@
         <v>0</v>
       </c>
       <c r="P66" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q66" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="R66" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B67">
         <v>46</v>
@@ -10803,18 +10809,18 @@
         <v>0</v>
       </c>
       <c r="P67" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Q67" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="R67" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B68">
         <v>46</v>
@@ -10859,18 +10865,18 @@
         <v>0</v>
       </c>
       <c r="P68" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="Q68" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="R68" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B69">
         <v>40</v>
@@ -10915,18 +10921,18 @@
         <v>0</v>
       </c>
       <c r="P69" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="Q69" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="R69" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B70">
         <v>40</v>
@@ -10971,18 +10977,18 @@
         <v>0</v>
       </c>
       <c r="P70" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="Q70" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="R70" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B71">
         <v>45</v>
@@ -11027,18 +11033,18 @@
         <v>0</v>
       </c>
       <c r="P71" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q71" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R71" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B72">
         <v>45</v>
@@ -11083,18 +11089,18 @@
         <v>0</v>
       </c>
       <c r="P72" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q72" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R72" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B73">
         <v>44</v>
@@ -11139,18 +11145,18 @@
         <v>0</v>
       </c>
       <c r="P73" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q73" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R73" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B74">
         <v>44</v>
@@ -11195,18 +11201,18 @@
         <v>0</v>
       </c>
       <c r="P74" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q74" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R74" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B75">
         <v>43</v>
@@ -11251,18 +11257,18 @@
         <v>0</v>
       </c>
       <c r="P75" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q75" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R75" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B76">
         <v>43</v>
@@ -11307,18 +11313,18 @@
         <v>0</v>
       </c>
       <c r="P76" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q76" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R76" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B77">
         <v>42</v>
@@ -11363,18 +11369,18 @@
         <v>0</v>
       </c>
       <c r="P77" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q77" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R77" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B78">
         <v>42</v>
@@ -11419,18 +11425,18 @@
         <v>0</v>
       </c>
       <c r="P78" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q78" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R78" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B79">
         <v>41</v>
@@ -11475,18 +11481,18 @@
         <v>0</v>
       </c>
       <c r="P79" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q79" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R79" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B80">
         <v>41</v>
@@ -11531,18 +11537,18 @@
         <v>0</v>
       </c>
       <c r="P80" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q80" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R80" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B81">
         <v>40</v>
@@ -11587,18 +11593,18 @@
         <v>0</v>
       </c>
       <c r="P81" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q81" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R81" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B82">
         <v>40</v>
@@ -11643,18 +11649,18 @@
         <v>0</v>
       </c>
       <c r="P82" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q82" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R82" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B83">
         <v>39</v>
@@ -11699,18 +11705,18 @@
         <v>0</v>
       </c>
       <c r="P83" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q83" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R83" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B84">
         <v>39</v>
@@ -11755,18 +11761,18 @@
         <v>0</v>
       </c>
       <c r="P84" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q84" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R84" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B85">
         <v>53</v>
@@ -11811,18 +11817,18 @@
         <v>0</v>
       </c>
       <c r="P85" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="Q85" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="R85" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B86">
         <v>53</v>
@@ -11867,18 +11873,18 @@
         <v>0</v>
       </c>
       <c r="P86" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="Q86" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="R86" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B87">
         <v>53</v>
@@ -11923,18 +11929,18 @@
         <v>0</v>
       </c>
       <c r="P87" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="Q87" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="R87" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B88">
         <v>14</v>
@@ -11979,18 +11985,18 @@
         <v>0</v>
       </c>
       <c r="P88" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q88" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R88" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B89">
         <v>19</v>
@@ -12035,18 +12041,18 @@
         <v>0</v>
       </c>
       <c r="P89" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q89" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R89" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B90">
         <v>24</v>
@@ -12091,18 +12097,18 @@
         <v>0</v>
       </c>
       <c r="P90" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q90" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R90" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B91">
         <v>29</v>
@@ -12147,18 +12153,18 @@
         <v>0</v>
       </c>
       <c r="P91" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q91" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R91" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B92">
         <v>34</v>
@@ -12203,18 +12209,18 @@
         <v>0</v>
       </c>
       <c r="P92" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q92" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R92" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B93">
         <v>39</v>
@@ -12259,18 +12265,18 @@
         <v>0</v>
       </c>
       <c r="P93" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q93" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R93" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B94">
         <v>44</v>
@@ -12315,18 +12321,18 @@
         <v>0</v>
       </c>
       <c r="P94" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q94" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R94" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B95">
         <v>49</v>
@@ -12371,18 +12377,18 @@
         <v>0</v>
       </c>
       <c r="P95" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q95" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R95" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B96">
         <v>54</v>
@@ -12427,18 +12433,18 @@
         <v>0</v>
       </c>
       <c r="P96" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q96" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R96" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B97">
         <v>59</v>
@@ -12483,18 +12489,18 @@
         <v>0</v>
       </c>
       <c r="P97" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q97" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R97" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B98">
         <v>64</v>
@@ -12539,18 +12545,18 @@
         <v>0</v>
       </c>
       <c r="P98" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q98" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R98" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B99">
         <v>69</v>
@@ -12595,18 +12601,18 @@
         <v>0</v>
       </c>
       <c r="P99" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q99" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R99" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B100">
         <v>74</v>
@@ -12651,13 +12657,13 @@
         <v>0</v>
       </c>
       <c r="P100" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Q100" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R100" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -12771,10 +12777,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12783,100 +12789,88 @@
     <col min="2" max="2" width="167.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>42327</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>42328</v>
-      </c>
-      <c r="B17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <v>42329</v>
+        <v>42327</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
         <v>50</v>
@@ -12884,10 +12878,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <v>42344</v>
+        <v>42328</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
         <v>50</v>
@@ -12895,10 +12889,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <v>42344</v>
+        <v>42329</v>
       </c>
       <c r="B20" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
@@ -12906,10 +12900,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <v>42371</v>
+        <v>42344</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
         <v>50</v>
@@ -12917,10 +12911,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>42607</v>
+        <v>42344</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>147</v>
       </c>
       <c r="C22" t="s">
         <v>50</v>
@@ -12928,57 +12922,57 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <v>42624</v>
+        <v>42371</v>
       </c>
       <c r="B23" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>142</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <v>42709</v>
+        <v>42607</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <v>42719</v>
+        <v>42624</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <v>42758</v>
+        <v>42709</v>
       </c>
       <c r="B26" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <v>42758</v>
+        <v>42719</v>
       </c>
       <c r="B27" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -12986,7 +12980,7 @@
         <v>42758</v>
       </c>
       <c r="B28" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C28" t="s">
         <v>50</v>
@@ -12997,7 +12991,7 @@
         <v>42758</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
@@ -13008,7 +13002,7 @@
         <v>42758</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C30" t="s">
         <v>50</v>
@@ -13016,10 +13010,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <v>42759</v>
+        <v>42758</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C31" t="s">
         <v>50</v>
@@ -13027,10 +13021,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
-        <v>42759</v>
+        <v>42758</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -13038,13 +13032,35 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
+        <v>42759</v>
+      </c>
+      <c r="B33" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>42759</v>
+      </c>
+      <c r="B34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
         <v>42760</v>
       </c>
-      <c r="B33" t="s">
-        <v>168</v>
-      </c>
-      <c r="C33" t="s">
-        <v>169</v>
+      <c r="B35" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>